<commit_message>
Proper parseing of the valgrind messages is a little more complex
sadly, this is slowing things down.
</commit_message>
<xml_diff>
--- a/leaks.xlsx
+++ b/leaks.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" r:id="Rb120cb7184e34fd5"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" r:id="R12a62db6f9c04e62"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -61,7 +61,7 @@
         <x:v>25957</x:v>
       </x:c>
       <x:c r="C3" t="n">
-        <x:v>0</x:v>
+        <x:v>25951</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
@@ -72,7 +72,7 @@
         <x:v>882960</x:v>
       </x:c>
       <x:c r="C4" t="n">
-        <x:v>0</x:v>
+        <x:v>888124</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -83,7 +83,7 @@
         <x:v>503301</x:v>
       </x:c>
       <x:c r="C5" t="n">
-        <x:v>0</x:v>
+        <x:v>473336</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
@@ -94,7 +94,7 @@
         <x:v>39136849</x:v>
       </x:c>
       <x:c r="C6" t="n">
-        <x:v>0</x:v>
+        <x:v>39198943</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
@@ -105,7 +105,7 @@
         <x:v>181383</x:v>
       </x:c>
       <x:c r="C7" t="n">
-        <x:v>0</x:v>
+        <x:v>229211</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
@@ -116,7 +116,7 @@
         <x:v>43638695</x:v>
       </x:c>
       <x:c r="C8" t="n">
-        <x:v>0</x:v>
+        <x:v>44188288</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
@@ -127,7 +127,7 @@
         <x:v>625728</x:v>
       </x:c>
       <x:c r="C9" t="n">
-        <x:v>0</x:v>
+        <x:v>625832</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
@@ -138,7 +138,7 @@
         <x:v>69028905</x:v>
       </x:c>
       <x:c r="C10" t="n">
-        <x:v>0</x:v>
+        <x:v>69036601</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>